<commit_message>
BigHomeWork1 - klaidų taisymas ir korekcijos
</commit_message>
<xml_diff>
--- a/BigHomeWork1/TūkstančioLaipsniai.xlsx
+++ b/BigHomeWork1/TūkstančioLaipsniai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\C_Sharp\GitHub\BigHomeWork1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B3036E-29B5-4575-86BE-6F04123C1384}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6766EA88-C4BF-47DD-980F-072D3FE668E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A1A84CFD-AF1C-4CE9-BCCE-2C8F80572B5F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A1A84CFD-AF1C-4CE9-BCCE-2C8F80572B5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Lapas1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="8">
   <si>
     <t>tūkstančių</t>
   </si>
@@ -34,6 +34,21 @@
   </si>
   <si>
     <t>tūkstančiai</t>
+  </si>
+  <si>
+    <t>Antras</t>
+  </si>
+  <si>
+    <t>Trečias</t>
+  </si>
+  <si>
+    <t>Pirmas</t>
+  </si>
+  <si>
+    <t>!1</t>
+  </si>
+  <si>
+    <t>.2-9.</t>
   </si>
 </sst>
 </file>
@@ -50,7 +65,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,8 +108,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -102,11 +129,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -114,6 +156,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Įprastas" xfId="0" builtinId="0"/>
@@ -428,19 +475,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D0551B5-4087-4C10-B8DF-18DA7A64F392}">
-  <dimension ref="E1:K68"/>
+  <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L49" sqref="L49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="15.140625" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D1" s="11"/>
       <c r="E1" s="3">
         <v>10000</v>
       </c>
@@ -453,22 +503,36 @@
       <c r="K1" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="8"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D2" s="11"/>
       <c r="E2" s="3">
         <v>11000</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="I2" s="1"/>
       <c r="J2" s="5">
         <v>101000</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="8"/>
+      <c r="M2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D3" s="11"/>
       <c r="E3" s="3">
         <v>12000</v>
       </c>
@@ -481,8 +545,12 @@
       <c r="K3" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D4" s="11"/>
       <c r="E4" s="3">
         <v>13000</v>
       </c>
@@ -495,8 +563,18 @@
       <c r="K4" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D5" s="11"/>
       <c r="E5" s="3">
         <v>14000</v>
       </c>
@@ -509,8 +587,25 @@
       <c r="K5" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="3">
         <v>15000</v>
       </c>
@@ -524,7 +619,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="11"/>
       <c r="E7" s="3">
         <v>16000</v>
       </c>
@@ -538,7 +641,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9">
+        <v>0</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="11"/>
       <c r="E8" s="3">
         <v>17000</v>
       </c>
@@ -551,8 +662,24 @@
       <c r="K8" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="M8" s="9"/>
+      <c r="N8" s="9">
+        <v>1</v>
+      </c>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="11"/>
       <c r="E9" s="3">
         <v>18000</v>
       </c>
@@ -565,8 +692,20 @@
       <c r="K9" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9">
+        <v>1</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C10" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="11"/>
       <c r="E10" s="3">
         <v>19000</v>
       </c>
@@ -579,8 +718,17 @@
       <c r="K10" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9">
+        <v>0</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D11" s="11"/>
       <c r="E11" s="2">
         <v>20000</v>
       </c>
@@ -593,8 +741,13 @@
       <c r="K11" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="8"/>
+      <c r="P11" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D12" s="11"/>
       <c r="E12" s="1">
         <v>21000</v>
       </c>
@@ -607,8 +760,9 @@
       <c r="K12" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E13">
         <v>22000</v>
       </c>
@@ -621,8 +775,9 @@
       <c r="K13" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E14">
         <v>23000</v>
       </c>
@@ -635,8 +790,9 @@
       <c r="K14" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E15">
         <v>24000</v>
       </c>
@@ -649,8 +805,9 @@
       <c r="K15" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E16">
         <v>25000</v>
       </c>
@@ -663,8 +820,9 @@
       <c r="K16" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E17">
         <v>26000</v>
       </c>
@@ -677,8 +835,9 @@
       <c r="K17" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E18">
         <v>27000</v>
       </c>
@@ -691,8 +850,9 @@
       <c r="K18" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E19">
         <v>28000</v>
       </c>
@@ -705,8 +865,9 @@
       <c r="K19" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="8"/>
+    </row>
+    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E20">
         <v>29000</v>
       </c>
@@ -719,8 +880,10 @@
       <c r="K20" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="8"/>
+    </row>
+    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D21" s="11"/>
       <c r="E21" s="2">
         <v>30000</v>
       </c>
@@ -733,22 +896,26 @@
       <c r="K21" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="8"/>
+    </row>
+    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D22" s="11"/>
       <c r="E22" s="1">
         <v>31000</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="I22" s="1"/>
       <c r="J22" s="5">
         <v>121000</v>
       </c>
       <c r="K22" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="8"/>
+    </row>
+    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E23">
         <v>32000</v>
       </c>
@@ -762,7 +929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E24">
         <v>33000</v>
       </c>
@@ -776,7 +943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E25">
         <v>34000</v>
       </c>
@@ -790,7 +957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E26">
         <v>35000</v>
       </c>
@@ -804,7 +971,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E27">
         <v>36000</v>
       </c>
@@ -818,7 +985,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E28">
         <v>37000</v>
       </c>
@@ -832,7 +999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E29">
         <v>38000</v>
       </c>
@@ -846,7 +1013,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E30">
         <v>39000</v>
       </c>
@@ -860,7 +1027,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D31" s="11"/>
       <c r="E31" s="2">
         <v>40000</v>
       </c>
@@ -873,22 +1041,26 @@
       <c r="K31" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L31" s="8"/>
+    </row>
+    <row r="32" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D32" s="11"/>
       <c r="E32" s="1">
         <v>41000</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="I32" s="1"/>
       <c r="J32" s="5">
         <v>131000</v>
       </c>
       <c r="K32" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L32" s="8"/>
+    </row>
+    <row r="33" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E33">
         <v>42000</v>
       </c>
@@ -902,7 +1074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E34">
         <v>43000</v>
       </c>
@@ -916,7 +1088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E35">
         <v>44000</v>
       </c>
@@ -930,7 +1102,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E36">
         <v>45000</v>
       </c>
@@ -944,7 +1116,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E37">
         <v>46000</v>
       </c>
@@ -958,7 +1130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E38">
         <v>47000</v>
       </c>
@@ -972,7 +1144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E39">
         <v>48000</v>
       </c>
@@ -986,7 +1158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E40">
         <v>49000</v>
       </c>
@@ -1000,7 +1172,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D41" s="11"/>
       <c r="E41" s="2">
         <v>50000</v>
       </c>
@@ -1013,22 +1186,25 @@
       <c r="K41" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L41" s="8"/>
+    </row>
+    <row r="42" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E42" s="1">
         <v>51000</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="I42" s="1"/>
       <c r="J42" s="6">
         <v>141000</v>
       </c>
       <c r="K42" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L42" s="8"/>
+    </row>
+    <row r="43" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E43">
         <v>52000</v>
       </c>
@@ -1042,7 +1218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E44">
         <v>53000</v>
       </c>
@@ -1056,7 +1232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E45">
         <v>54000</v>
       </c>
@@ -1070,7 +1246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E46">
         <v>55000</v>
       </c>
@@ -1084,7 +1260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E47">
         <v>56000</v>
       </c>
@@ -1098,7 +1274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E48">
         <v>57000</v>
       </c>
@@ -1112,7 +1288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E49">
         <v>58000</v>
       </c>
@@ -1126,7 +1302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J50" s="6">
         <v>149000</v>
       </c>
@@ -1134,23 +1310,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J51" s="6">
         <v>150000</v>
       </c>
       <c r="K51" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L51" s="8"/>
+    </row>
+    <row r="52" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="I52" s="1"/>
       <c r="J52" s="6">
         <v>151000</v>
       </c>
       <c r="K52" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L52" s="8"/>
+    </row>
+    <row r="53" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J53" s="6">
         <v>152000</v>
       </c>
@@ -1158,7 +1337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J54" s="6">
         <v>153000</v>
       </c>
@@ -1166,7 +1345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J55" s="6">
         <v>154000</v>
       </c>
@@ -1174,7 +1353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J56" s="6">
         <v>155000</v>
       </c>
@@ -1182,7 +1361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J57" s="6">
         <v>156000</v>
       </c>
@@ -1190,7 +1369,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J58" s="6">
         <v>157000</v>
       </c>
@@ -1198,7 +1377,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J59" s="6">
         <v>158000</v>
       </c>
@@ -1206,7 +1385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J60" s="6">
         <v>159000</v>
       </c>
@@ -1214,7 +1393,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J61" s="6">
         <v>160000</v>
       </c>
@@ -1222,7 +1401,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J62" s="6">
         <v>161000</v>
       </c>
@@ -1230,7 +1409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J63" s="6">
         <v>162000</v>
       </c>
@@ -1238,7 +1417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J64" s="6">
         <v>163000</v>
       </c>

</xml_diff>